<commit_message>
removed auth from fast api article dump
</commit_message>
<xml_diff>
--- a/Bulk_Article_dump/ADdata.xlsx
+++ b/Bulk_Article_dump/ADdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>domain</t>
   </si>
@@ -22,22 +22,10 @@
     <t>tld</t>
   </si>
   <si>
-    <t>content_suitableanswers</t>
-  </si>
-  <si>
-    <t>com</t>
-  </si>
-  <si>
     <t>answergenius</t>
   </si>
   <si>
     <t>net</t>
-  </si>
-  <si>
-    <t>content_getsmartinsights</t>
-  </si>
-  <si>
-    <t>content_ww1_smartanswers</t>
   </si>
 </sst>
 </file>
@@ -384,7 +372,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -411,28 +399,16 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1"/>
@@ -441,18 +417,6 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>